<commit_message>
remove /assets/js/user/analysis.js's visial part, which already changed into /controller/graphic
</commit_message>
<xml_diff>
--- a/tes_file/Book2.xlsx
+++ b/tes_file/Book2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t xml:space="preserve">收款方</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">aaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fff</t>
   </si>
   <si>
     <t xml:space="preserve">ccc</t>
@@ -58,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -157,12 +161,12 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -181,7 +185,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>500</v>
@@ -189,10 +193,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>100</v>
@@ -200,10 +204,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>200</v>
@@ -211,7 +215,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -222,10 +226,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>200</v>

</xml_diff>